<commit_message>
Effettuato lo sbroglio per le modifiche apportate
</commit_message>
<xml_diff>
--- a/ESECUTIVI/LP22-301-0.xlsx
+++ b/ESECUTIVI/LP22-301-0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Utenti\00.Lavori in corso\METALTRONICA\22-301-0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Utenti\00.Lavori in corso\METALTRONICA\22-301-0 (SCHEDA SERVIZI 2_02_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AF120138-EE35-4B62-9A13-E2D69B52E5DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E6B854-43C1-433B-A49B-C2B1787182C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="22-301-0" sheetId="1" r:id="rId1"/>
@@ -127,9 +127,6 @@
     <t>SMD0603</t>
   </si>
   <si>
-    <t>C8,C9,C10,C11,C12,C13,C14,C15,C16,C17,C18,C19,C20,C24,C25,C29,C30,C31,C32,C33,C34,C35,C36,C37,C39,C40,C49,C50,C51,C52,C53,C55,C56,C59,C63,C68,C73,C77,C80,C85,C87,C88,C89,C90,C91,C93,C94,C97,C98,C99,C100,C101,C102,C103,C104,C105,C107,C108,C110,C115,C116,C117,C118,C119,C120,C121</t>
-  </si>
-  <si>
     <t>MLCC - SMD/SMT 50V 0.1uF X7R 0603 10%</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
     <t>50V, X7R</t>
   </si>
   <si>
-    <t>C21,C22,C23,C26,C27,C28</t>
-  </si>
-  <si>
     <t>MLCC - SMD/SMT 50V  68pF COG (NP0)  0603 2%</t>
   </si>
   <si>
@@ -775,9 +769,6 @@
     <t>115mA</t>
   </si>
   <si>
-    <t>L2,L3,L5,L6,L7,L8,L9,L10,L11,L12,L13,L14,L20,L21,L22,L23,L25,L26,L27,L28,L29,L30</t>
-  </si>
-  <si>
     <t>Ferrite Bead</t>
   </si>
   <si>
@@ -1012,27 +1003,15 @@
     <t>10K</t>
   </si>
   <si>
-    <t>R25,R32</t>
-  </si>
-  <si>
     <t>33R</t>
   </si>
   <si>
-    <t>R26,R33</t>
-  </si>
-  <si>
     <t>120R</t>
   </si>
   <si>
-    <t>R27,R28,R31,R34,R35,R38</t>
-  </si>
-  <si>
     <t>470R</t>
   </si>
   <si>
-    <t>R29,R30,R36,R37</t>
-  </si>
-  <si>
     <t>60R</t>
   </si>
   <si>
@@ -1234,9 +1213,6 @@
     <t>30V Nominal</t>
   </si>
   <si>
-    <t>TVS7,TVS8,TVS9,TVS10,TVS11,TVS12,TVS13,TVS14,TVS15,TVS16,TVS17,TVS19,TVS20,TVS21,TVS22,TVS23,TVS24,TVS25,TVS26,TVS27,TVS28,TVS29,TVS30,TVS31,TVS32,TVS33,TVS34,TVS35,TVS36,TVS37,TVS40,TVS42</t>
-  </si>
-  <si>
     <t>SMBJ5A</t>
   </si>
   <si>
@@ -1309,9 +1285,6 @@
     <t>1.8 to 5.5V</t>
   </si>
   <si>
-    <t>U13,U14</t>
-  </si>
-  <si>
     <t>CAN TRANSCEIVER</t>
   </si>
   <si>
@@ -1525,13 +1498,40 @@
     <t>LISTA PARTI SCHEDA 22-301-0</t>
   </si>
   <si>
-    <t>DATA 20/9/2022</t>
+    <t>DATA 2/2/2024</t>
+  </si>
+  <si>
+    <t>C8,C9,C10,C11,C12,C13,C14,C15,C16,C17,C18,C19,C20,C30,C31,C32,C33,C34,C35,C36,C37,C39,C40,C49,C50,C51,C52,C53,C55,C56,C59,C63,C68,C73,C77,C80,C85,C87,C88,C89,C90,C91,C93,C94,C97,C98,C99,C100,C101,C102,C103,C104,C105,C107,C108,C110,C115,C116,C117,C118,C119,C120,C121</t>
+  </si>
+  <si>
+    <t>C21,C22,C23</t>
+  </si>
+  <si>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R27,R28,R31</t>
+  </si>
+  <si>
+    <t>R29,R30</t>
+  </si>
+  <si>
+    <t>TVS7,TVS8,TVS9,TVS10,TVS11,TVS12,TVS13,TVS14,TVS15,TVS16,TVS17,TVS19,TVS20,TVS21,TVS22,TVS27,TVS28,TVS29,TVS30,TVS31,TVS32,TVS33,TVS34,TVS35,TVS36,TVS37,TVS40,TVS42</t>
+  </si>
+  <si>
+    <t>U13</t>
+  </si>
+  <si>
+    <t>L7,L8,L9,L10,L11,L12,L13,L14,L20,L21,L22,L23,L25,L26,L27,L28,L29,L30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2442,11 +2442,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2467,13 +2467,13 @@
   <sheetData>
     <row r="1" spans="1:11" s="5" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="G1" s="6" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="K1" s="7"/>
     </row>
@@ -2622,27 +2622,27 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="210" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>4</v>
       </c>
       <c r="B7" s="13">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C7" s="14" t="s">
+        <v>492</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="E7" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="F7" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="G7" s="13" t="s">
         <v>37</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>38</v>
       </c>
       <c r="H7" s="15" t="s">
         <v>32</v>
@@ -2654,7 +2654,7 @@
         <v>33</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2662,22 +2662,22 @@
         <v>5</v>
       </c>
       <c r="B8" s="13">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8" s="14" t="s">
+        <v>493</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="F8" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="G8" s="13" t="s">
         <v>42</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>44</v>
       </c>
       <c r="H8" s="15" t="s">
         <v>32</v>
@@ -2700,19 +2700,19 @@
         <v>20</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H9" s="15" t="s">
         <v>32</v>
@@ -2724,7 +2724,7 @@
         <v>33</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2735,31 +2735,31 @@
         <v>7</v>
       </c>
       <c r="C10" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="F10" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="G10" s="13" t="s">
         <v>51</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>53</v>
       </c>
       <c r="H10" s="15" t="s">
         <v>32</v>
       </c>
       <c r="I10" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="K10" s="14" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -2770,31 +2770,31 @@
         <v>2</v>
       </c>
       <c r="C11" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="F11" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="G11" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="H11" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="I11" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="J11" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="K11" s="14" t="s">
         <v>63</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2805,31 +2805,31 @@
         <v>4</v>
       </c>
       <c r="C12" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="F12" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="G12" s="13" t="s">
         <v>68</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="H12" s="15" t="s">
         <v>32</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2840,31 +2840,31 @@
         <v>1</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D13" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="G13" s="13" t="s">
         <v>68</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="H13" s="15" t="s">
         <v>32</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2875,16 +2875,16 @@
         <v>1</v>
       </c>
       <c r="C14" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="F14" s="16" t="s">
         <v>74</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>76</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>23</v>
@@ -2897,7 +2897,7 @@
         <v>33</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2908,16 +2908,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="F15" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>81</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>23</v>
@@ -2930,7 +2930,7 @@
         <v>33</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2941,16 +2941,16 @@
         <v>1</v>
       </c>
       <c r="C16" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="F16" s="16" t="s">
         <v>83</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>85</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>23</v>
@@ -2976,16 +2976,16 @@
         <v>1</v>
       </c>
       <c r="C17" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="F17" s="16" t="s">
         <v>87</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>89</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>32</v>
@@ -3000,7 +3000,7 @@
         <v>26</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -3011,31 +3011,31 @@
         <v>1</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H18" s="15" t="s">
         <v>32</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J18" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3046,19 +3046,19 @@
         <v>2</v>
       </c>
       <c r="C19" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="F19" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="G19" s="13" t="s">
         <v>97</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>99</v>
       </c>
       <c r="H19" s="15" t="s">
         <v>32</v>
@@ -3070,7 +3070,7 @@
         <v>33</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3081,31 +3081,31 @@
         <v>1</v>
       </c>
       <c r="C20" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="F20" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="G20" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="H20" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="J20" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="H20" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>106</v>
-      </c>
       <c r="K20" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
@@ -3116,28 +3116,28 @@
         <v>19</v>
       </c>
       <c r="C21" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="F21" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="G21" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="H21" s="15" t="s">
         <v>110</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>112</v>
       </c>
       <c r="I21" s="15" t="s">
         <v>25</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K21" s="14"/>
     </row>
@@ -3149,28 +3149,28 @@
         <v>6</v>
       </c>
       <c r="C22" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="E22" s="15" t="s">
+      <c r="G22" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F22" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>117</v>
-      </c>
       <c r="H22" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I22" s="15" t="s">
         <v>25</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K22" s="14"/>
     </row>
@@ -3182,28 +3182,28 @@
         <v>1</v>
       </c>
       <c r="C23" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="D23" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="E23" s="15" t="s">
+      <c r="G23" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="F23" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>121</v>
-      </c>
       <c r="H23" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I23" s="15" t="s">
         <v>25</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K23" s="14"/>
     </row>
@@ -3215,31 +3215,31 @@
         <v>2</v>
       </c>
       <c r="C24" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="F24" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="G24" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="H24" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="F24" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="G24" s="13" t="s">
+      <c r="I24" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="J24" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="I24" s="15" t="s">
+      <c r="K24" s="14" t="s">
         <v>127</v>
-      </c>
-      <c r="J24" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="K24" s="14" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -3250,31 +3250,31 @@
         <v>3</v>
       </c>
       <c r="C25" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="F25" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="G25" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="H25" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="F25" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="G25" s="13" t="s">
+      <c r="I25" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="J25" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="I25" s="15" t="s">
+      <c r="K25" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="J25" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="K25" s="14" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -3285,31 +3285,31 @@
         <v>4</v>
       </c>
       <c r="C26" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="G26" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="D26" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="E26" s="15" t="s">
+      <c r="H26" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="I26" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="F26" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="G26" s="13" t="s">
+      <c r="J26" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="H26" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="I26" s="15" t="s">
+      <c r="K26" s="14" t="s">
         <v>141</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="K26" s="14" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -3320,31 +3320,31 @@
         <v>5</v>
       </c>
       <c r="C27" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="E27" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="F27" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="G27" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="H27" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="I27" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="F27" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="G27" s="13" t="s">
+      <c r="J27" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="H27" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="I27" s="15" t="s">
+      <c r="K27" s="14" t="s">
         <v>148</v>
-      </c>
-      <c r="J27" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="K27" s="14" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -3355,31 +3355,31 @@
         <v>1</v>
       </c>
       <c r="C28" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="F28" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="G28" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="H28" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="J28" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="K28" s="14" t="s">
         <v>155</v>
-      </c>
-      <c r="H28" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="J28" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="K28" s="14" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -3390,31 +3390,31 @@
         <v>1</v>
       </c>
       <c r="C29" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="E29" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="F29" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="G29" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="H29" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="F29" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="G29" s="13" t="s">
+      <c r="I29" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="H29" s="15" t="s">
+      <c r="J29" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="I29" s="15" t="s">
+      <c r="K29" s="14" t="s">
         <v>163</v>
-      </c>
-      <c r="J29" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="K29" s="14" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -3425,28 +3425,28 @@
         <v>2</v>
       </c>
       <c r="C30" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="E30" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="F30" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="G30" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="H30" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="I30" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="J30" s="15" t="s">
         <v>170</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="I30" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="J30" s="15" t="s">
-        <v>172</v>
       </c>
       <c r="K30" s="14"/>
     </row>
@@ -3458,28 +3458,28 @@
         <v>2</v>
       </c>
       <c r="C31" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="F31" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="G31" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="E31" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="F31" s="16" t="s">
+      <c r="H31" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="I31" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="J31" s="15" t="s">
         <v>176</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="J31" s="15" t="s">
-        <v>178</v>
       </c>
       <c r="K31" s="14"/>
     </row>
@@ -3491,18 +3491,18 @@
         <v>6</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D32" s="14"/>
       <c r="E32" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F32" s="16"/>
       <c r="G32" s="13"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K32" s="14"/>
     </row>
@@ -3514,28 +3514,28 @@
         <v>1</v>
       </c>
       <c r="C33" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="E33" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="F33" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="G33" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="H33" s="15" t="s">
         <v>185</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="H33" s="15" t="s">
-        <v>187</v>
       </c>
       <c r="I33" s="15" t="s">
         <v>17</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K33" s="14"/>
     </row>
@@ -3547,26 +3547,26 @@
         <v>2</v>
       </c>
       <c r="C34" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E34" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="F34" s="16" t="s">
         <v>190</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="F34" s="16" t="s">
-        <v>192</v>
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I34" s="15" t="s">
         <v>17</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K34" s="14"/>
     </row>
@@ -3578,28 +3578,28 @@
         <v>1</v>
       </c>
       <c r="C35" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="E35" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="F35" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="G35" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="F35" s="16" t="s">
-        <v>197</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>198</v>
-      </c>
       <c r="H35" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I35" s="15" t="s">
         <v>17</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K35" s="14"/>
     </row>
@@ -3611,28 +3611,28 @@
         <v>1</v>
       </c>
       <c r="C36" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="E36" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="F36" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="G36" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="F36" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>204</v>
-      </c>
       <c r="H36" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I36" s="15" t="s">
         <v>17</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K36" s="14"/>
     </row>
@@ -3644,28 +3644,28 @@
         <v>1</v>
       </c>
       <c r="C37" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="E37" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="F37" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="G37" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="F37" s="16" t="s">
+      <c r="H37" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="G37" s="13" t="s">
+      <c r="I37" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="H37" s="15" t="s">
+      <c r="J37" s="15" t="s">
         <v>211</v>
-      </c>
-      <c r="I37" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="J37" s="15" t="s">
-        <v>213</v>
       </c>
       <c r="K37" s="14"/>
     </row>
@@ -3677,31 +3677,31 @@
         <v>2</v>
       </c>
       <c r="C38" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="E38" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="F38" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="G38" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="H38" s="15" t="s">
         <v>216</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>218</v>
       </c>
       <c r="I38" s="15" t="s">
         <v>17</v>
       </c>
       <c r="J38" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K38" s="14" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -3712,31 +3712,31 @@
         <v>1</v>
       </c>
       <c r="C39" s="14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="E39" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="F39" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="G39" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="E39" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>224</v>
-      </c>
       <c r="H39" s="15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I39" s="15" t="s">
         <v>17</v>
       </c>
       <c r="J39" s="15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K39" s="14" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -3747,10 +3747,10 @@
         <v>1</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E40" s="15">
         <v>61200621621</v>
@@ -3759,16 +3759,16 @@
         <v>61200621621</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="I40" s="15" t="s">
         <v>17</v>
       </c>
       <c r="J40" s="15" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K40" s="14"/>
     </row>
@@ -3780,28 +3780,28 @@
         <v>1</v>
       </c>
       <c r="C41" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="E41" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="F41" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="G41" s="13" t="s">
         <v>234</v>
       </c>
-      <c r="F41" s="16" t="s">
+      <c r="H41" s="15" t="s">
         <v>235</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="H41" s="15" t="s">
-        <v>237</v>
       </c>
       <c r="I41" s="15" t="s">
         <v>17</v>
       </c>
       <c r="J41" s="15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K41" s="14"/>
     </row>
@@ -3813,20 +3813,20 @@
         <v>1</v>
       </c>
       <c r="C42" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="E42" s="15" t="s">
         <v>239</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="E42" s="15" t="s">
-        <v>241</v>
       </c>
       <c r="F42" s="16"/>
       <c r="G42" s="13"/>
       <c r="H42" s="15"/>
       <c r="I42" s="15"/>
       <c r="J42" s="15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="K42" s="14"/>
     </row>
@@ -3838,57 +3838,57 @@
         <v>2</v>
       </c>
       <c r="C43" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="E43" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="F43" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="G43" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="H43" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="F43" s="16" t="s">
-        <v>245</v>
-      </c>
-      <c r="G43" s="13" t="s">
+      <c r="I43" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="J43" s="15" t="s">
         <v>246</v>
       </c>
-      <c r="H43" s="15" t="s">
+      <c r="K43" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="I43" s="15" t="s">
-        <v>245</v>
-      </c>
-      <c r="J43" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="K43" s="14" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>41</v>
       </c>
       <c r="B44" s="13">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C44" s="14" t="s">
+        <v>500</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="F44" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="G44" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="E44" s="15" t="s">
-        <v>252</v>
-      </c>
-      <c r="F44" s="16" t="s">
-        <v>253</v>
-      </c>
-      <c r="G44" s="13" t="s">
-        <v>254</v>
-      </c>
       <c r="H44" s="15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I44" s="15" t="s">
         <v>33</v>
@@ -3897,7 +3897,7 @@
         <v>33</v>
       </c>
       <c r="K44" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -3908,28 +3908,28 @@
         <v>4</v>
       </c>
       <c r="C45" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="G45" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="H45" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="I45" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="J45" s="15" t="s">
         <v>258</v>
-      </c>
-      <c r="F45" s="16" t="s">
-        <v>258</v>
-      </c>
-      <c r="G45" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="H45" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="I45" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="J45" s="15" t="s">
-        <v>261</v>
       </c>
       <c r="K45" s="14"/>
     </row>
@@ -3941,31 +3941,31 @@
         <v>1</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="F46" s="16">
         <v>7447773220</v>
       </c>
       <c r="G46" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="H46" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="I46" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="J46" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="K46" s="14" t="s">
         <v>265</v>
-      </c>
-      <c r="H46" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="I46" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="J46" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="K46" s="14" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3976,31 +3976,31 @@
         <v>2</v>
       </c>
       <c r="C47" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="F47" s="16" t="s">
         <v>269</v>
       </c>
-      <c r="D47" s="14" t="s">
+      <c r="G47" s="13" t="s">
         <v>270</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="H47" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="F47" s="16" t="s">
+      <c r="I47" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="G47" s="13" t="s">
+      <c r="J47" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="H47" s="15" t="s">
+      <c r="K47" s="14" t="s">
         <v>274</v>
-      </c>
-      <c r="I47" s="15" t="s">
-        <v>275</v>
-      </c>
-      <c r="J47" s="15" t="s">
-        <v>276</v>
-      </c>
-      <c r="K47" s="14" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -4011,31 +4011,31 @@
         <v>3</v>
       </c>
       <c r="C48" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="E48" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="G48" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="H48" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="E48" s="15" t="s">
+      <c r="I48" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="F48" s="16" t="s">
-        <v>280</v>
-      </c>
-      <c r="G48" s="13" t="s">
+      <c r="J48" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="H48" s="15" t="s">
+      <c r="K48" s="14" t="s">
         <v>282</v>
-      </c>
-      <c r="I48" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="J48" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="K48" s="14" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -4046,31 +4046,31 @@
         <v>4</v>
       </c>
       <c r="C49" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="F49" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="H49" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="I49" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="J49" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="K49" s="14" t="s">
         <v>286</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>287</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="G49" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="H49" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="I49" s="15" t="s">
-        <v>283</v>
-      </c>
-      <c r="J49" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="K49" s="14" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="105" x14ac:dyDescent="0.25">
@@ -4081,31 +4081,31 @@
         <v>2</v>
       </c>
       <c r="C50" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="E50" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="G50" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="H50" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="D50" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="E50" s="15" t="s">
+      <c r="I50" s="15" t="s">
         <v>291</v>
       </c>
-      <c r="F50" s="16" t="s">
-        <v>291</v>
-      </c>
-      <c r="G50" s="13" t="s">
+      <c r="J50" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="H50" s="15" t="s">
+      <c r="K50" s="14" t="s">
         <v>293</v>
-      </c>
-      <c r="I50" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="J50" s="15" t="s">
-        <v>295</v>
-      </c>
-      <c r="K50" s="14" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -4116,31 +4116,31 @@
         <v>2</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="E51" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="F51" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="G51" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="H51" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="I51" s="15" t="s">
         <v>291</v>
       </c>
-      <c r="F51" s="16" t="s">
-        <v>291</v>
-      </c>
-      <c r="G51" s="13" t="s">
-        <v>292</v>
-      </c>
-      <c r="H51" s="15" t="s">
-        <v>293</v>
-      </c>
-      <c r="I51" s="15" t="s">
-        <v>294</v>
-      </c>
       <c r="J51" s="15" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="K51" s="14" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -4151,28 +4151,28 @@
         <v>1</v>
       </c>
       <c r="C52" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="F52" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="G52" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="H52" s="15" t="s">
         <v>302</v>
-      </c>
-      <c r="F52" s="16" t="s">
-        <v>303</v>
-      </c>
-      <c r="G52" s="13" t="s">
-        <v>304</v>
-      </c>
-      <c r="H52" s="15" t="s">
-        <v>305</v>
       </c>
       <c r="I52" s="15" t="s">
         <v>17</v>
       </c>
       <c r="J52" s="15" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="K52" s="14"/>
     </row>
@@ -4184,28 +4184,28 @@
         <v>2</v>
       </c>
       <c r="C53" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="E53" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="F53" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="G53" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="E53" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="F53" s="16" t="s">
-        <v>310</v>
-      </c>
-      <c r="G53" s="13" t="s">
-        <v>311</v>
-      </c>
       <c r="H53" s="15" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="I53" s="15" t="s">
         <v>17</v>
       </c>
       <c r="J53" s="15" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="K53" s="14"/>
     </row>
@@ -4217,28 +4217,28 @@
         <v>1</v>
       </c>
       <c r="C54" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="F54" s="16" t="s">
+        <v>312</v>
+      </c>
+      <c r="G54" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="H54" s="15" t="s">
         <v>314</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="F54" s="16" t="s">
-        <v>315</v>
-      </c>
-      <c r="G54" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="H54" s="15" t="s">
-        <v>317</v>
       </c>
       <c r="I54" s="15" t="s">
         <v>17</v>
       </c>
       <c r="J54" s="15" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="K54" s="14"/>
     </row>
@@ -4250,22 +4250,22 @@
         <v>19</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G55" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I55" s="15" t="s">
         <v>33</v>
@@ -4283,28 +4283,28 @@
         <v>21</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G56" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I56" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J56" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K56" s="14"/>
     </row>
@@ -4316,22 +4316,22 @@
         <v>35</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F57" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G57" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I57" s="15" t="s">
         <v>33</v>
@@ -4349,22 +4349,22 @@
         <v>11</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F58" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G58" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I58" s="15" t="s">
         <v>33</v>
@@ -4379,25 +4379,25 @@
         <v>56</v>
       </c>
       <c r="B59" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>329</v>
+        <v>494</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G59" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I59" s="15" t="s">
         <v>33</v>
@@ -4412,25 +4412,25 @@
         <v>57</v>
       </c>
       <c r="B60" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>331</v>
+        <v>495</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E60" s="15" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I60" s="15" t="s">
         <v>33</v>
@@ -4440,30 +4440,30 @@
       </c>
       <c r="K60" s="14"/>
     </row>
-    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="13">
         <v>58</v>
       </c>
       <c r="B61" s="13">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>333</v>
+        <v>496</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E61" s="15" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H61" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I61" s="15" t="s">
         <v>33</v>
@@ -4478,25 +4478,25 @@
         <v>59</v>
       </c>
       <c r="B62" s="13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>335</v>
+        <v>497</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E62" s="15" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H62" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I62" s="15" t="s">
         <v>33</v>
@@ -4514,22 +4514,22 @@
         <v>5</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F63" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H63" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I63" s="15" t="s">
         <v>33</v>
@@ -4547,22 +4547,22 @@
         <v>6</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G64" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I64" s="15" t="s">
         <v>33</v>
@@ -4580,22 +4580,22 @@
         <v>9</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H65" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I65" s="15" t="s">
         <v>33</v>
@@ -4613,31 +4613,31 @@
         <v>17</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="E66" s="15" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="F66" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H66" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I66" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J66" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K66" s="14" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
@@ -4648,22 +4648,22 @@
         <v>2</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="D67" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E67" s="15" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="F67" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H67" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I67" s="15" t="s">
         <v>33</v>
@@ -4681,22 +4681,22 @@
         <v>6</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E68" s="15" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="F68" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H68" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I68" s="15" t="s">
         <v>33</v>
@@ -4714,22 +4714,22 @@
         <v>1</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E69" s="15" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="F69" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G69" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I69" s="15" t="s">
         <v>33</v>
@@ -4747,22 +4747,22 @@
         <v>1</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E70" s="15" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="F70" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H70" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I70" s="15" t="s">
         <v>33</v>
@@ -4780,22 +4780,22 @@
         <v>1</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="F71" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H71" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I71" s="15" t="s">
         <v>33</v>
@@ -4813,22 +4813,22 @@
         <v>1</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="F72" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H72" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I72" s="15" t="s">
         <v>33</v>
@@ -4846,22 +4846,22 @@
         <v>1</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E73" s="15" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="F73" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H73" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I73" s="15" t="s">
         <v>33</v>
@@ -4879,22 +4879,22 @@
         <v>1</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E74" s="15" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="F74" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G74" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H74" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I74" s="15" t="s">
         <v>33</v>
@@ -4912,22 +4912,22 @@
         <v>1</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="E75" s="15" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="F75" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G75" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H75" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I75" s="15" t="s">
         <v>25</v>
@@ -4945,22 +4945,22 @@
         <v>1</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E76" s="15" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="F76" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G76" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H76" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I76" s="15" t="s">
         <v>25</v>
@@ -4969,7 +4969,7 @@
         <v>26</v>
       </c>
       <c r="K76" s="14" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -4980,31 +4980,31 @@
         <v>1</v>
       </c>
       <c r="C77" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>362</v>
+      </c>
+      <c r="F77" s="16" t="s">
+        <v>363</v>
+      </c>
+      <c r="G77" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="H77" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="I77" s="15" t="s">
+        <v>365</v>
+      </c>
+      <c r="J77" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="K77" s="14" t="s">
         <v>367</v>
-      </c>
-      <c r="D77" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="E77" s="15" t="s">
-        <v>369</v>
-      </c>
-      <c r="F77" s="16" t="s">
-        <v>370</v>
-      </c>
-      <c r="G77" s="13" t="s">
-        <v>371</v>
-      </c>
-      <c r="H77" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="I77" s="15" t="s">
-        <v>372</v>
-      </c>
-      <c r="J77" s="15" t="s">
-        <v>373</v>
-      </c>
-      <c r="K77" s="14" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -5015,22 +5015,22 @@
         <v>2</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E78" s="15" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="F78" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H78" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I78" s="15" t="s">
         <v>33</v>
@@ -5048,31 +5048,31 @@
         <v>1</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="E79" s="15" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="F79" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G79" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I79" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J79" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K79" s="14" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -5083,22 +5083,22 @@
         <v>5</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E80" s="15" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="F80" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G80" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H80" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I80" s="15" t="s">
         <v>25</v>
@@ -5107,7 +5107,7 @@
         <v>26</v>
       </c>
       <c r="K80" s="14" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -5118,22 +5118,22 @@
         <v>1</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="D81" s="14" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E81" s="15" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="F81" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G81" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H81" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I81" s="15" t="s">
         <v>25</v>
@@ -5142,7 +5142,7 @@
         <v>26</v>
       </c>
       <c r="K81" s="14" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -5153,22 +5153,22 @@
         <v>2</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E82" s="15" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="F82" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G82" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H82" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I82" s="15" t="s">
         <v>25</v>
@@ -5177,7 +5177,7 @@
         <v>26</v>
       </c>
       <c r="K82" s="14" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -5188,31 +5188,31 @@
         <v>2</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="D83" s="14" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="E83" s="15" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="F83" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G83" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H83" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I83" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J83" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K83" s="14" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -5223,31 +5223,31 @@
         <v>1</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="E84" s="15" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="F84" s="16" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="G84" s="13" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="H84" s="15" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="I84" s="15" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="J84" s="15" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="K84" s="14" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -5258,22 +5258,22 @@
         <v>2</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E85" s="15" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="F85" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G85" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H85" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I85" s="15" t="s">
         <v>25</v>
@@ -5282,7 +5282,7 @@
         <v>26</v>
       </c>
       <c r="K85" s="14" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -5293,22 +5293,22 @@
         <v>1</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E86" s="15" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="F86" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H86" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I86" s="15" t="s">
         <v>25</v>
@@ -5317,7 +5317,7 @@
         <v>26</v>
       </c>
       <c r="K86" s="14" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
@@ -5328,22 +5328,22 @@
         <v>1</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E87" s="15" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="F87" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H87" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I87" s="15" t="s">
         <v>25</v>
@@ -5352,7 +5352,7 @@
         <v>26</v>
       </c>
       <c r="K87" s="14" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="88" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -5363,19 +5363,19 @@
         <v>11</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="E88" s="15" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="F88" s="16" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="G88" s="13" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="H88" s="15" t="b">
         <v>1</v>
@@ -5384,7 +5384,7 @@
         <v>17</v>
       </c>
       <c r="J88" s="15" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="K88" s="14"/>
     </row>
@@ -5396,64 +5396,64 @@
         <v>40</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="E89" s="15" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="F89" s="16" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="G89" s="13" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="H89" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I89" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J89" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K89" s="14" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A90" s="13">
         <v>87</v>
       </c>
       <c r="B90" s="13">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>403</v>
+        <v>498</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="E90" s="15" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="F90" s="16" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="G90" s="13"/>
       <c r="H90" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I90" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J90" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K90" s="14" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -5464,28 +5464,28 @@
         <v>16</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="E91" s="15" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="F91" s="16" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="G91" s="13" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="H91" s="15" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="I91" s="15" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="J91" s="15" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="K91" s="14"/>
     </row>
@@ -5497,28 +5497,28 @@
         <v>35</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="E92" s="15" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="F92" s="16" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="G92" s="13" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="H92" s="15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I92" s="15" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="J92" s="15" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="K92" s="14"/>
     </row>
@@ -5530,31 +5530,31 @@
         <v>1</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="E93" s="15" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="F93" s="16" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="G93" s="13" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="H93" s="15" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="I93" s="15" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="J93" s="15" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="K93" s="14" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
@@ -5562,34 +5562,34 @@
         <v>91</v>
       </c>
       <c r="B94" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>428</v>
+        <v>499</v>
       </c>
       <c r="D94" s="14" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="E94" s="15" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="F94" s="16" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="G94" s="13" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="H94" s="15" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="I94" s="15" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="J94" s="15" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="K94" s="14" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -5600,31 +5600,31 @@
         <v>4</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="E95" s="15" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="F95" s="16" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="G95" s="13" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="H95" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I95" s="15" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="J95" s="15" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="K95" s="14" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
     </row>
     <row r="96" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -5635,31 +5635,31 @@
         <v>1</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="E96" s="15" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="F96" s="16" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="G96" s="13" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="H96" s="15" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="I96" s="15" t="s">
         <v>17</v>
       </c>
       <c r="J96" s="15" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="K96" s="14" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
@@ -5670,28 +5670,28 @@
         <v>1</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="D97" s="14" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="E97" s="15" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="F97" s="16" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="G97" s="13" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="H97" s="15" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="I97" s="15" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="J97" s="15" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="K97" s="14"/>
     </row>
@@ -5703,31 +5703,31 @@
         <v>1</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="E98" s="15" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="F98" s="16" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="G98" s="13" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
       <c r="H98" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I98" s="15" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="J98" s="15" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="K98" s="14" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
@@ -5738,28 +5738,28 @@
         <v>1</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="E99" s="15" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="F99" s="16" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="G99" s="13" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="H99" s="15" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="I99" s="15" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="J99" s="15" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="K99" s="14"/>
     </row>
@@ -5771,31 +5771,31 @@
         <v>1</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="E100" s="15" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="F100" s="16" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="G100" s="13" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
       <c r="H100" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I100" s="15" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="J100" s="15" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="K100" s="14" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
     </row>
     <row r="101" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -5806,29 +5806,29 @@
         <v>1</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="E101" s="15" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="F101" s="16" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="G101" s="13"/>
       <c r="H101" s="15" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="I101" s="15" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="J101" s="15" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="K101" s="14" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -5839,28 +5839,28 @@
         <v>2</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="E102" s="15" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="F102" s="16" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="G102" s="13" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="H102" s="15" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="I102" s="15" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="J102" s="15" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="K102" s="14"/>
     </row>
@@ -5872,28 +5872,28 @@
         <v>1</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="E103" s="15" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="F103" s="16" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="G103" s="13" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="H103" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I103" s="15" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="J103" s="15" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="K103" s="14"/>
     </row>
@@ -5905,18 +5905,18 @@
         <v>8</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="15" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="F104" s="16"/>
       <c r="G104" s="13"/>
       <c r="H104" s="15"/>
       <c r="I104" s="15"/>
       <c r="J104" s="15" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="K104" s="14"/>
     </row>
@@ -5928,31 +5928,31 @@
         <v>1</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="D105" s="14" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="E105" s="15" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="F105" s="16" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="G105" s="13" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="H105" s="15" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="I105" s="15" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
       <c r="J105" s="15" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="K105" s="14" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
     </row>
   </sheetData>

</xml_diff>